<commit_message>
Initial implementation of full flow
</commit_message>
<xml_diff>
--- a/src/lib/datasource/telas-checklist.xlsx
+++ b/src/lib/datasource/telas-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zmil425/Documents/Git/Blended Learning Checklist/src/lib/datasource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0618F39-3B7B-2745-B315-E8DF675B86F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC49451D-786F-C04C-8527-A18306679E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{393FAFA0-95E4-B343-A34C-FE2CEA66C230}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">STANDARD 1: The design of the online learning environment design supports a positive learner experience. </t>
-  </si>
-  <si>
     <t>1.1. The online learning environment is inclusive.</t>
   </si>
   <si>
@@ -344,9 +341,6 @@
   </si>
   <si>
     <t>Check for instructions provided to students on how their feedback should be submitted and what it would be used for. You may want to look for the description of purpose in a feedback or evaluation survey, or the introduction of a completion checklist for learning materials, a discussion thread opening, or task description of a reflection journal, etc.</t>
-  </si>
-  <si>
-    <t>STANDARD 2: The online environment design supports learning.</t>
   </si>
   <si>
     <t>2.1. The navigation and layout of the online learning environment is functional, consistent and intuitive.</t>
@@ -514,9 +508,6 @@
     <t>Check the overall content presentation to see if it is easy to navigate around the learning resources provided.</t>
   </si>
   <si>
-    <t>STANDARD 3: The online learning environment includes administrative, technical and learning information and support.</t>
-  </si>
-  <si>
     <t>3.1. Links to relevant services, information and policies are provided.</t>
   </si>
   <si>
@@ -646,9 +637,6 @@
     <t>3.5.3. Information on how to interpret learning analytics is provided.</t>
   </si>
   <si>
-    <t>STANDARD 4: The online environment includes learner and teacher interactions that are designed to support and progress learning.</t>
-  </si>
-  <si>
     <t>4.1. Opportunities for learner-to-learner interactions are provided.</t>
   </si>
   <si>
@@ -761,9 +749,6 @@
     </r>
   </si>
   <si>
-    <t>STANDARD 5: Learning and assessment tasks engage learners through planned learning experiences and feedback.</t>
-  </si>
-  <si>
     <t>5.1. The aims, learning outcomes, schedule of learning and assessment tasks, and participation expectations are provided.</t>
   </si>
   <si>
@@ -930,9 +915,6 @@
     <t>5.5.2. Information about feedback (e.g. timing, format, interpretation, use) is provided.</t>
   </si>
   <si>
-    <t>STANDARD 6: Learning and assessment tasks leverage the affordances of digital technologies and support the development of digital literacies.</t>
-  </si>
-  <si>
     <t>6.1. Learning and assessment tasks are supported by relevant digital technology.</t>
   </si>
   <si>
@@ -954,9 +936,6 @@
     <t>6.2.2. Opportunities to develop and demonstrate digital literacies are appropriately scaffolded.</t>
   </si>
   <si>
-    <t>STANDARD 7: Learning resources are available, functional, inclusive and are compliant with copyright and attribution requirements.</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.1. Learning resources are available and functional. </t>
   </si>
   <si>
@@ -994,9 +973,6 @@
   </si>
   <si>
     <t>7.3.3. Learning resources are contextualized to more than one global region.</t>
-  </si>
-  <si>
-    <t>STANDARD 8: Learning resources are relevant and support learner engagement.</t>
   </si>
   <si>
     <t>8.1. Learning resources are relevant.</t>
@@ -1064,6 +1040,30 @@
   </si>
   <si>
     <t>Your learning environment should include relevant resources with contextual explanations and utilize a variety of digital technologies and media to support engagement. Ensure resources are presented in multiple modalities to cater to different learning preferences.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The design of the online learning environment design supports a positive learner experience. </t>
+  </si>
+  <si>
+    <t>The online environment design supports learning.</t>
+  </si>
+  <si>
+    <t>The online learning environment includes administrative, technical and learning information and support.</t>
+  </si>
+  <si>
+    <t>The online environment includes learner and teacher interactions that are designed to support and progress learning.</t>
+  </si>
+  <si>
+    <t>Learning and assessment tasks engage learners through planned learning experiences and feedback.</t>
+  </si>
+  <si>
+    <t>Learning and assessment tasks leverage the affordances of digital technologies and support the development of digital literacies.</t>
+  </si>
+  <si>
+    <t>Learning resources are available, functional, inclusive and are compliant with copyright and attribution requirements.</t>
+  </si>
+  <si>
+    <t>Learning resources are relevant and support learner engagement.</t>
   </si>
 </sst>
 </file>
@@ -1693,11 +1693,38 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1705,33 +1732,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2092,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5334662-9413-C34F-BABB-F5B50512B303}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83:B85"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2141,1343 +2141,1325 @@
     </row>
     <row r="2" spans="1:12" ht="42" x14ac:dyDescent="0.2">
       <c r="A2" s="60" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="56" t="s">
-        <v>193</v>
-      </c>
-      <c r="C2" s="54" t="s">
+      <c r="D2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="G2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="I2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="J2" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="K2" s="39" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>17</v>
       </c>
       <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.2">
       <c r="A3" s="61"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="G3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="40" t="s">
+      <c r="J3" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="K3" s="39" t="s">
         <v>21</v>
-      </c>
-      <c r="K3" s="39" t="s">
-        <v>22</v>
       </c>
       <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:12" ht="42" x14ac:dyDescent="0.2">
       <c r="A4" s="61"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="54" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="57"/>
+      <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="G4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="41" t="s">
+      <c r="J4" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="K4" s="39" t="s">
         <v>27</v>
-      </c>
-      <c r="K4" s="39" t="s">
-        <v>28</v>
       </c>
       <c r="L4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="39" x14ac:dyDescent="0.2">
       <c r="A5" s="61"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="G5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="39" t="s">
+      <c r="K5" s="39" t="s">
         <v>31</v>
-      </c>
-      <c r="K5" s="39" t="s">
-        <v>32</v>
       </c>
       <c r="L5" s="34"/>
     </row>
     <row r="6" spans="1:12" ht="77" x14ac:dyDescent="0.2">
       <c r="A6" s="61"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="G6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="43" t="s">
+      <c r="J6" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="K6" s="44" t="s">
         <v>36</v>
-      </c>
-      <c r="K6" s="44" t="s">
-        <v>37</v>
       </c>
       <c r="L6" s="34"/>
     </row>
     <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="61"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="54" t="s">
+      <c r="B7" s="66"/>
+      <c r="C7" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="57"/>
+      <c r="E7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="G7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="45" t="s">
+      <c r="J7" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="K7" s="46" t="s">
         <v>42</v>
-      </c>
-      <c r="K7" s="46" t="s">
-        <v>43</v>
       </c>
       <c r="L7" s="34"/>
     </row>
     <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="61"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="G8" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="I8" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="J8" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="K8" s="48" t="s">
         <v>48</v>
-      </c>
-      <c r="K8" s="48" t="s">
-        <v>49</v>
       </c>
       <c r="L8" s="34"/>
     </row>
     <row r="9" spans="1:12" ht="78" x14ac:dyDescent="0.2">
       <c r="A9" s="61"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="G9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="49" t="s">
+      <c r="J9" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="K9" s="48" t="s">
         <v>53</v>
-      </c>
-      <c r="K9" s="48" t="s">
-        <v>54</v>
       </c>
       <c r="L9" s="34"/>
     </row>
     <row r="10" spans="1:12" ht="52" x14ac:dyDescent="0.2">
       <c r="A10" s="61"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="G10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" s="39" t="s">
+      <c r="K10" s="46" t="s">
         <v>57</v>
-      </c>
-      <c r="K10" s="46" t="s">
-        <v>58</v>
       </c>
       <c r="L10" s="34"/>
     </row>
     <row r="11" spans="1:12" ht="42" x14ac:dyDescent="0.2">
       <c r="A11" s="61"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="54" t="s">
+      <c r="B11" s="66"/>
+      <c r="C11" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="E11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="G11" t="s">
         <v>62</v>
-      </c>
-      <c r="G11" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="84" x14ac:dyDescent="0.2">
       <c r="A12" s="61"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
       <c r="E12" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="35" t="s">
-        <v>65</v>
-      </c>
       <c r="G12" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="56" x14ac:dyDescent="0.2">
       <c r="A13" s="62"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
       <c r="E13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="35" t="s">
-        <v>67</v>
-      </c>
       <c r="G13" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="60" t="s">
+        <v>194</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="57"/>
+      <c r="E14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="56" t="s">
-        <v>194</v>
-      </c>
-      <c r="C14" s="54" t="s">
+      <c r="F14" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="5" t="s">
+      <c r="G14" s="21" t="s">
         <v>70</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="28" x14ac:dyDescent="0.2">
       <c r="A15" s="61"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
       <c r="E15" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="26" x14ac:dyDescent="0.2">
       <c r="A16" s="61"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
       <c r="E16" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28" x14ac:dyDescent="0.2">
       <c r="A17" s="61"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F17" s="53" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="42" x14ac:dyDescent="0.2">
       <c r="A18" s="61"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
       <c r="E18" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="28" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G19" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="70" x14ac:dyDescent="0.2">
       <c r="A20" s="61"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
       <c r="E20" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="42" x14ac:dyDescent="0.2">
       <c r="A21" s="61"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="54" t="s">
+      <c r="B21" s="66"/>
+      <c r="C21" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="57"/>
+      <c r="E21" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="12" t="s">
+      <c r="G21" s="23" t="s">
         <v>87</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28" x14ac:dyDescent="0.2">
       <c r="A22" s="61"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
       <c r="E22" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="56" x14ac:dyDescent="0.2">
       <c r="A23" s="61"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
       <c r="E23" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F23" s="53" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="62"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
       <c r="E24" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="76" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="57"/>
+      <c r="E25" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="56" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="54"/>
-      <c r="E25" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>99</v>
-      </c>
       <c r="G25" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A26" s="61"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
       <c r="E26" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="61"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
       <c r="E27" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="61"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="54" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="54"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="57"/>
       <c r="E28" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="61"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
       <c r="E29" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="61"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="54"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="57"/>
       <c r="E30" s="12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="61"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
       <c r="E31" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="61"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" s="54"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="57"/>
       <c r="E32" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A33" s="61"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="55"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="59"/>
       <c r="E33" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="61"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="54"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="57"/>
       <c r="E34" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="61"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="55"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="59"/>
       <c r="E35" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="61"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="54"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="57"/>
       <c r="E36" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="61"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" s="55"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="59"/>
       <c r="E37" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="61"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="54"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="57"/>
       <c r="E38" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="62"/>
-      <c r="B39" s="58"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
       <c r="E39" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="56" t="s">
         <v>196</v>
       </c>
-      <c r="C40" s="54" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" s="54"/>
+      <c r="B40" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="C40" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="57"/>
       <c r="E40" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="61"/>
-      <c r="B41" s="57"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="55"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="59"/>
       <c r="E41" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="61"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="54"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="57"/>
       <c r="E42" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="61"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
       <c r="E43" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A44" s="61"/>
-      <c r="B44" s="57"/>
-      <c r="C44" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="D44" s="54"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="57"/>
       <c r="E44" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A45" s="61"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="55"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F45" s="14"/>
       <c r="G45" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="61"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="54"/>
+      <c r="B46" s="66"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="57"/>
       <c r="E46" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F46" s="14"/>
       <c r="G46" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="61"/>
-      <c r="B47" s="57"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
       <c r="E47" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F47" s="14"/>
       <c r="G47" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="61"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="D48" s="54"/>
+      <c r="B48" s="66"/>
+      <c r="C48" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" s="57"/>
       <c r="E48" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F48" s="14"/>
       <c r="G48" s="27" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A49" s="61"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="55"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="59"/>
       <c r="E49" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F49" s="14"/>
       <c r="G49" s="28" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="61"/>
-      <c r="B50" s="57"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="54"/>
+      <c r="B50" s="66"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="57"/>
       <c r="E50" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F50" s="14"/>
       <c r="G50" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="62"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
+      <c r="B51" s="67"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
       <c r="E51" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F51" s="14"/>
       <c r="G51" s="30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="60" t="s">
-        <v>139</v>
-      </c>
-      <c r="B52" s="56" t="s">
         <v>197</v>
       </c>
-      <c r="C52" s="54" t="s">
-        <v>140</v>
-      </c>
-      <c r="D52" s="54"/>
+      <c r="B52" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="57"/>
       <c r="E52" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F52" s="14"/>
       <c r="G52" s="17" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="61"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
+      <c r="B53" s="66"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
       <c r="E53" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A54" s="61"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="D54" s="54"/>
+      <c r="B54" s="66"/>
+      <c r="C54" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" s="57"/>
       <c r="E54" s="12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F54" s="14"/>
       <c r="G54" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="39" x14ac:dyDescent="0.2">
       <c r="A55" s="61"/>
-      <c r="B55" s="57"/>
-      <c r="C55" s="59"/>
-      <c r="D55" s="55"/>
+      <c r="B55" s="66"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="59"/>
       <c r="E55" s="11" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F55" s="14"/>
       <c r="G55" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="61"/>
-      <c r="B56" s="57"/>
-      <c r="C56" s="59"/>
-      <c r="D56" s="54"/>
+      <c r="B56" s="66"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="57"/>
       <c r="E56" s="8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F56" s="14"/>
       <c r="G56" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="61"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="59"/>
-      <c r="D57" s="55"/>
+      <c r="B57" s="66"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="59"/>
       <c r="E57" s="8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F57" s="14"/>
       <c r="G57" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="61"/>
-      <c r="B58" s="57"/>
-      <c r="C58" s="55"/>
-      <c r="D58" s="54"/>
+      <c r="B58" s="66"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="57"/>
       <c r="E58" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F58" s="14"/>
       <c r="G58" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="61"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="54" t="s">
-        <v>151</v>
-      </c>
-      <c r="D59" s="55"/>
+      <c r="B59" s="66"/>
+      <c r="C59" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" s="59"/>
       <c r="E59" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F59" s="14"/>
       <c r="G59" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A60" s="61"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="55"/>
-      <c r="D60" s="54"/>
+      <c r="B60" s="66"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="57"/>
       <c r="E60" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F60" s="14"/>
       <c r="G60" s="17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A61" s="61"/>
-      <c r="B61" s="57"/>
-      <c r="C61" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="D61" s="55"/>
+      <c r="B61" s="66"/>
+      <c r="C61" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="59"/>
       <c r="E61" s="12" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F61" s="14"/>
       <c r="G61" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="61"/>
-      <c r="B62" s="57"/>
-      <c r="C62" s="59"/>
-      <c r="D62" s="54"/>
+      <c r="B62" s="66"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="57"/>
       <c r="E62" s="11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F62" s="14"/>
       <c r="G62" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A63" s="61"/>
-      <c r="B63" s="57"/>
-      <c r="C63" s="59"/>
-      <c r="D63" s="55"/>
+      <c r="B63" s="66"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="59"/>
       <c r="E63" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F63" s="14"/>
       <c r="G63" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A64" s="61"/>
-      <c r="B64" s="57"/>
-      <c r="C64" s="59"/>
-      <c r="D64" s="54"/>
+      <c r="B64" s="66"/>
+      <c r="C64" s="58"/>
+      <c r="D64" s="57"/>
       <c r="E64" s="11" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F64" s="14"/>
       <c r="G64" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="26" x14ac:dyDescent="0.2">
       <c r="A65" s="61"/>
-      <c r="B65" s="57"/>
-      <c r="C65" s="55"/>
-      <c r="D65" s="55"/>
+      <c r="B65" s="66"/>
+      <c r="C65" s="59"/>
+      <c r="D65" s="59"/>
       <c r="E65" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F65" s="14"/>
       <c r="G65" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="61"/>
-      <c r="B66" s="57"/>
-      <c r="C66" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="D66" s="54"/>
+      <c r="B66" s="66"/>
+      <c r="C66" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="D66" s="57"/>
       <c r="E66" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="62"/>
-      <c r="B67" s="58"/>
-      <c r="C67" s="55"/>
-      <c r="D67" s="55"/>
+      <c r="B67" s="67"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="59"/>
       <c r="E67" s="9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F67" s="14"/>
       <c r="G67" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="60" t="s">
-        <v>164</v>
-      </c>
-      <c r="B68" s="56" t="s">
         <v>198</v>
       </c>
-      <c r="C68" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="D68" s="67"/>
+      <c r="B68" s="65" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="D68" s="54"/>
       <c r="E68" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F68" s="14"/>
       <c r="G68" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="61"/>
-      <c r="B69" s="57"/>
-      <c r="C69" s="59"/>
-      <c r="D69" s="66"/>
+      <c r="B69" s="66"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="55"/>
       <c r="E69" s="11" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F69" s="14"/>
       <c r="G69" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="61"/>
-      <c r="B70" s="57"/>
-      <c r="C70" s="64"/>
-      <c r="D70" s="66"/>
+      <c r="B70" s="66"/>
+      <c r="C70" s="63"/>
+      <c r="D70" s="55"/>
       <c r="E70" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F70" s="14"/>
       <c r="G70" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="61"/>
-      <c r="B71" s="57"/>
-      <c r="C71" s="63" t="s">
-        <v>169</v>
-      </c>
-      <c r="D71" s="66"/>
+      <c r="B71" s="66"/>
+      <c r="C71" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="D71" s="55"/>
       <c r="E71" s="12" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F71" s="14"/>
     </row>
     <row r="72" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="62"/>
-      <c r="B72" s="58"/>
-      <c r="C72" s="55"/>
-      <c r="D72" s="66"/>
+      <c r="B72" s="67"/>
+      <c r="C72" s="59"/>
+      <c r="D72" s="55"/>
       <c r="E72" s="6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F72" s="14"/>
     </row>
     <row r="73" spans="1:7" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="60" t="s">
-        <v>172</v>
-      </c>
-      <c r="B73" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="C73" s="54" t="s">
-        <v>173</v>
-      </c>
-      <c r="D73" s="66"/>
+      <c r="B73" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="C73" s="57" t="s">
+        <v>166</v>
+      </c>
+      <c r="D73" s="55"/>
       <c r="E73" s="5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F73" s="14"/>
       <c r="G73" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="61"/>
-      <c r="B74" s="57"/>
-      <c r="C74" s="59"/>
-      <c r="D74" s="66"/>
+      <c r="B74" s="66"/>
+      <c r="C74" s="58"/>
+      <c r="D74" s="55"/>
       <c r="E74" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="F74" s="14"/>
       <c r="G74" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="61"/>
-      <c r="B75" s="57"/>
-      <c r="C75" s="59"/>
-      <c r="D75" s="66"/>
+      <c r="B75" s="66"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="55"/>
       <c r="E75" s="8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F75" s="14"/>
       <c r="G75" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="61"/>
-      <c r="B76" s="57"/>
-      <c r="C76" s="59"/>
-      <c r="D76" s="66"/>
+      <c r="B76" s="66"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="55"/>
       <c r="E76" s="11" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F76" s="14"/>
       <c r="G76" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="61"/>
-      <c r="B77" s="57"/>
-      <c r="C77" s="55"/>
-      <c r="D77" s="65"/>
+      <c r="B77" s="66"/>
+      <c r="C77" s="59"/>
+      <c r="D77" s="56"/>
       <c r="E77" s="6" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F77" s="14"/>
       <c r="G77" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="61"/>
-      <c r="B78" s="57"/>
-      <c r="C78" s="54" t="s">
-        <v>179</v>
-      </c>
-      <c r="D78" s="54"/>
+      <c r="B78" s="66"/>
+      <c r="C78" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="D78" s="57"/>
       <c r="E78" s="7" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F78" s="14"/>
       <c r="G78" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="61"/>
-      <c r="B79" s="57"/>
-      <c r="C79" s="55"/>
-      <c r="D79" s="55"/>
+      <c r="B79" s="66"/>
+      <c r="C79" s="59"/>
+      <c r="D79" s="59"/>
       <c r="E79" s="6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F79" s="14"/>
     </row>
     <row r="80" spans="1:7" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="61"/>
-      <c r="B80" s="57"/>
-      <c r="C80" s="54" t="s">
-        <v>182</v>
-      </c>
-      <c r="D80" s="67"/>
+      <c r="B80" s="66"/>
+      <c r="C80" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="D80" s="54"/>
       <c r="E80" s="12" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F80" s="14"/>
       <c r="G80" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="61"/>
-      <c r="B81" s="57"/>
-      <c r="C81" s="59"/>
-      <c r="D81" s="66"/>
+      <c r="B81" s="66"/>
+      <c r="C81" s="58"/>
+      <c r="D81" s="55"/>
       <c r="E81" s="11" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F81" s="14"/>
       <c r="G81" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="62"/>
-      <c r="B82" s="58"/>
-      <c r="C82" s="55"/>
-      <c r="D82" s="66"/>
+      <c r="B82" s="67"/>
+      <c r="C82" s="59"/>
+      <c r="D82" s="55"/>
       <c r="E82" s="6" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F82" s="14"/>
       <c r="G82" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="60" t="s">
-        <v>186</v>
-      </c>
-      <c r="B83" s="56" t="s">
         <v>200</v>
       </c>
+      <c r="B83" s="65" t="s">
+        <v>192</v>
+      </c>
       <c r="C83" s="4" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D83" s="51"/>
       <c r="E83" s="13" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="F83" s="14"/>
       <c r="G83" s="15" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="61"/>
-      <c r="B84" s="57"/>
-      <c r="C84" s="63" t="s">
-        <v>190</v>
-      </c>
-      <c r="D84" s="67"/>
+      <c r="B84" s="66"/>
+      <c r="C84" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="D84" s="54"/>
       <c r="E84" s="12" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F84" s="14"/>
     </row>
     <row r="85" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="61"/>
-      <c r="B85" s="57"/>
-      <c r="C85" s="55"/>
-      <c r="D85" s="65"/>
+      <c r="B85" s="66"/>
+      <c r="C85" s="59"/>
+      <c r="D85" s="56"/>
       <c r="E85" s="11" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F85" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="D73:D77"/>
-    <mergeCell ref="D80:D82"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="A14:A24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="A25:A39"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="A40:A51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C61:C65"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="A52:A67"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="A68:A72"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C73:C77"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="A73:A82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="D64:D65"/>
     <mergeCell ref="C84:C85"/>
     <mergeCell ref="A83:A85"/>
     <mergeCell ref="D38:D39"/>
@@ -3494,29 +3476,47 @@
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="D84:D85"/>
+    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C73:C77"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="A73:A82"/>
+    <mergeCell ref="B52:B67"/>
+    <mergeCell ref="B68:B72"/>
+    <mergeCell ref="B73:B82"/>
+    <mergeCell ref="A40:A51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C61:C65"/>
+    <mergeCell ref="A52:A67"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="A14:A24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A25:A39"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="B14:B24"/>
     <mergeCell ref="B25:B39"/>
-    <mergeCell ref="B40:B51"/>
-    <mergeCell ref="B52:B67"/>
-    <mergeCell ref="B68:B72"/>
-    <mergeCell ref="B73:B82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="D73:D77"/>
+    <mergeCell ref="D80:D82"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C71:C72"/>
     <mergeCell ref="D71:D72"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>

<commit_message>
App is now functional
All three modes are now usable at some level, although they are missing some features.
</commit_message>
<xml_diff>
--- a/src/lib/datasource/telas-checklist.xlsx
+++ b/src/lib/datasource/telas-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zmil425/Documents/Git/Blended Learning Checklist/src/lib/datasource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC49451D-786F-C04C-8527-A18306679E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDA7913-7DBB-BB48-BC24-F358485DD48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{393FAFA0-95E4-B343-A34C-FE2CEA66C230}"/>
   </bookViews>
@@ -83,15 +83,9 @@
     <t>Description</t>
   </si>
   <si>
-    <t>1.1. The online learning environment is inclusive.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The online learning environment is respectful and promotes the acceptance and value of all people. </t>
   </si>
   <si>
-    <t>1.1.1. Language used is consistently appropriate and inclusive (including consistent tone, voice, person).</t>
-  </si>
-  <si>
     <t>Skim the entire learning package quickly to see if language throughout the course is culturally appropriate and respectful of the diversity (age, cultural, linguistic, gender and sexuality, disability, religion, etc.) of UoA's people.</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>These success indicators are part of the canvas baseline practice project and should be present in all canvas courses.</t>
   </si>
   <si>
-    <t>1.1.2. The online learning environment contains evidence that diverse perspectives are respected.</t>
-  </si>
-  <si>
     <t>Check if various viewpoints, sources, theories from Aotearoa and beyond are presentated and discussed.</t>
   </si>
   <si>
@@ -120,12 +111,6 @@
   </si>
   <si>
     <t>A positive student experience throughout the course</t>
-  </si>
-  <si>
-    <t>1.2. The online learning environment functions across devices and platforms.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.2.1. The online learning environment is responsive across different contemporary devices (e.g. screen size adjusting automatically).</t>
   </si>
   <si>
     <t>Check if the course displays properly on a range of electronic devices, e.g  a desktop computer, a laptop, a tablet, and a smartphone. The more devices, the better as a course may look fine on a tablet but not on a phone screen or vice versa.</t>
@@ -141,9 +126,6 @@
 (potential incorporated into SJ?)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1.2.2. The online learning environment and integrated technology are compatible across multiple platforms and operating systems.</t>
-  </si>
-  <si>
     <t>Check if the course can be accessed on different platforms e.g., Microsoft, Android, Macintosh etc., and operating systems, e.g., Windows, iOS, Linux, etc.</t>
   </si>
   <si>
@@ -151,9 +133,6 @@
   </si>
   <si>
     <t>Cultural Responsive Pedagogy is about making learning relevant and effective for all learners.</t>
-  </si>
-  <si>
-    <t>1.2.3. The online learning environment and integrated technology are compatible with contemporary browsers.</t>
   </si>
   <si>
     <t>Access the course using different browsers to see if there are any problems loading or viewing it. Use as many browsers as possible, including Chrome, Firefox, Safari, and Internet Explorer, etc.</t>
@@ -170,6 +149,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Involves authentic learning – the use of examples that connect students to the material. See  </t>
     </r>
@@ -185,12 +165,6 @@
     </r>
   </si>
   <si>
-    <t>1.3. Online learning environment meets appropriate accessibility standards.</t>
-  </si>
-  <si>
-    <t>1.3.1. Site, content and activities meet a contemporary set of accessibility standards/guidelines (e.g. accessible font, contrasting colour).</t>
-  </si>
-  <si>
     <t>Will we reference using UDOIT here?
 Link to https://teachwell.auckland.ac.nz/resources/design-for-accessibility/</t>
   </si>
@@ -206,6 +180,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Emphasising the importance of getting to know our students – their needs, experience, ability and talent – and ‘us’. See </t>
     </r>
@@ -221,9 +196,6 @@
     </r>
   </si>
   <si>
-    <t>1.3.2. External tools and applications adhere to accessibility standards (e.g. Turnitin, VoiceThread, Echo360, SPSS, Padlet).</t>
-  </si>
-  <si>
     <t xml:space="preserve">Check if external tools and applications adhere to accessibility standards </t>
   </si>
   <si>
@@ -241,6 +213,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Collaborative learning approaches – group/team based learning, peer review activities, co-creation of learning content and more. See</t>
     </r>
@@ -250,12 +223,10 @@
         <sz val="12"/>
         <color rgb="FF467886"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> https://teachwell.auckland.ac.nz/signature-pedagogies/relational-learning/students-peers/</t>
     </r>
-  </si>
-  <si>
-    <t>1.3.3. Files are appropriately optimised for screen readers, consistently named, then labelled by type and size.</t>
   </si>
   <si>
     <t>Check if the course site is optimised for screen readers. The following link contains examples of problems that may make it hard for screen readers to work efficiently: https://www.washington.edu/accesscomputing/AU/v2/problems.html 
@@ -273,6 +244,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Students learning to learn and developing their academic identity and citizenship. See </t>
     </r>
@@ -282,12 +254,10 @@
         <sz val="12"/>
         <color rgb="FF467886"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://teachwell.auckland.ac.nz/signature-pedagogies/relational-learning/students-selves/</t>
     </r>
-  </si>
-  <si>
-    <t>1.3.4. Alternate formats are made available for multimedia (e.g. images and alternate texts, subtitling for video or audio, transcripts for video and audio).</t>
   </si>
   <si>
     <t>Check if multimedia content is provided in different formats to ensure that options are available to meet users’ needs and preferences. For example, whether photos have an accompanied text description, and audio or video recordings have subtitles and transcripts in case students did not or could not listen or watch.</t>
@@ -301,6 +271,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Involves work-integrated learning or community-based learning. See</t>
     </r>
@@ -316,37 +287,19 @@
     </r>
   </si>
   <si>
-    <t>1.4. Learners have opportunities to provide feedback.</t>
-  </si>
-  <si>
     <t>Opportunities are provided within the course for students to share feedback, with explicit information on how feedback will be collected and used.</t>
   </si>
   <si>
-    <t>1.4.1. Learners have opportunities to provide immediate feedback (e.g. thumbs up/down, stars, flagging).</t>
-  </si>
-  <si>
     <t>Check if students can provide immediate feedback after they engage with learning materials provided in the course site. For example, students might be invited to provide feedback in the Discussion Forum, Announcements, Introduction or Modules sections of the course.</t>
   </si>
   <si>
     <t>I think we said we might leave this out, as no options in Canvas for thumbs up, marking a task as completed, etc.</t>
   </si>
   <si>
-    <t>1.4.2. Learners have opportunities to provide feedback at different points in time (e.g. surveys polls, signposting).</t>
-  </si>
-  <si>
     <t>Check if there are any instructions or encouragement for students to provide feedback to teaching staff at different points of time, i.e., in different weeks at the beginning, middle and end of the course. You may also want to look for links to background surveys, reminders to complete course evaluation, discussion threads, reflection journals or even a quick feedback page in the weekly lecture/tutorial slides.The feedback can be of any form, e.g., orally or in writing, and various formats, e.g., via email, in Discussion Forum, feedback survey, etc.</t>
   </si>
   <si>
-    <t>1.4.3. Learners are informed about how their feedback is going to be collected and used.</t>
-  </si>
-  <si>
     <t>Check for instructions provided to students on how their feedback should be submitted and what it would be used for. You may want to look for the description of purpose in a feedback or evaluation survey, or the introduction of a completion checklist for learning materials, a discussion thread opening, or task description of a reflection journal, etc.</t>
-  </si>
-  <si>
-    <t>2.1. The navigation and layout of the online learning environment is functional, consistent and intuitive.</t>
-  </si>
-  <si>
-    <t>2.1.1. The navigation is useable and functional.</t>
   </si>
   <si>
     <t xml:space="preserve">Check if you can navigate through the menus, tabs, or pages of the course easily and efficiently. </t>
@@ -358,6 +311,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">CBP
 </t>
@@ -368,12 +322,10 @@
         <sz val="9"/>
         <color rgb="FF009999"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>SJ</t>
     </r>
-  </si>
-  <si>
-    <t>2.1.2. Instructions on how to navigate the site and where to find learning activities are provided.</t>
   </si>
   <si>
     <t xml:space="preserve">Check for instructions on the key content areas and where to find them. These may be provided in the welcome announcement or introduction section of the course, in text, or part of an intro video. </t>
@@ -395,13 +347,7 @@
     </r>
   </si>
   <si>
-    <t>2.1.3.  There is a consistent style guide (e.g. heading hierarchies, bulleted or numbered lists are consistent and tables only used for data).</t>
-  </si>
-  <si>
     <t>Skim quickly through the course  to see if it is presented in a consistent style across the sections.</t>
-  </si>
-  <si>
-    <t>2.1.4. All links and embedded resources are functional (i.e. not dead).</t>
   </si>
   <si>
     <r>
@@ -431,22 +377,10 @@
     <t>Check if there are explicit instructions on whether learning resources are accessible right on the course site or elsewhere, e.g. on the library, the publisher’s website or a bookstore.  Such instructions may be found at the beginning of the section for learning materials, introduction to the course, announcements.</t>
   </si>
   <si>
-    <t>2.1.6. When learners are directed to external resources it opens in a new window/tab</t>
-  </si>
-  <si>
     <t>Check all the external resources, such as embedded links, to see if they open in a new window or different tab from the one learners are viewing.</t>
   </si>
   <si>
-    <t>2.1.7. The channel(s) of communication for learners is articulated (e.g. dates, notices, updates and reminders).</t>
-  </si>
-  <si>
     <t>Check if all the channels that will be used for communicating with learners have been described. This may be in the Announcement, Introduction, Discussion forum and Assessment sections. The information may also be provided in the slides of the first lesson or welcome and course introduction video. Check for information about how long they should wait for a lecturer’s email response or when assessment results will become available, for example.</t>
-  </si>
-  <si>
-    <t>2.2. The online learning environment is logically sequenced and organised.</t>
-  </si>
-  <si>
-    <t>2.2.1. A summary is provided that gives an overview of the learning sequence/design.</t>
   </si>
   <si>
     <t>Check if an overview of the learning sequence or design is provided or summarised in the course site. For example, this may be a table describing the weekly content or topics, or a few sentences briefing the course structure.</t>
@@ -458,6 +392,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">CBP </t>
     </r>
@@ -467,18 +402,13 @@
         <sz val="9"/>
         <color rgb="FFFFC000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>CE</t>
     </r>
   </si>
   <si>
-    <t>2.2.2. The sequence of learning (i.e. order/flow) is logical.</t>
-  </si>
-  <si>
     <t>Skim the learning sequence to see if the content or topics are scaffolded coherently and build upon previous learning.</t>
-  </si>
-  <si>
-    <t>2.2.3. The content is divided into manageable segments that are appropriately labelled.</t>
   </si>
   <si>
     <r>
@@ -502,52 +432,10 @@
     </r>
   </si>
   <si>
-    <t>2.2.4. The content is organised to enhance ease of navigation.</t>
-  </si>
-  <si>
     <t>Check the overall content presentation to see if it is easy to navigate around the learning resources provided.</t>
   </si>
   <si>
-    <t>3.1. Links to relevant services, information and policies are provided.</t>
-  </si>
-  <si>
-    <t>3.1.1. Links to academic support services and resources are provided.</t>
-  </si>
-  <si>
     <t>Check if there are links to academic support services and learning resources in the course.</t>
-  </si>
-  <si>
-    <t>3.1.2. Links to up-to-date, relevant policies (e.g. academic integrity, copyright, assessment procedures) are provided.</t>
-  </si>
-  <si>
-    <t>3.1.3. Links to up-to-date, relevant institutional services (e.g. library, learner support) are provided.</t>
-  </si>
-  <si>
-    <t>3.2. Clear instructions for accessing technical support resources are provided.</t>
-  </si>
-  <si>
-    <t>3.2.1. Clear instructions for accessing technical support contacts are provided.</t>
-  </si>
-  <si>
-    <t>3.2.2. Instructions for accessing technical support services and resources are easy to find.</t>
-  </si>
-  <si>
-    <t>3.3. Clear and consistent instructions/guides for using the technology are provided.</t>
-  </si>
-  <si>
-    <t>3.3.1. The minimum technologies required to be successful are specified.</t>
-  </si>
-  <si>
-    <t>3.3.2. Learners are provided with instructions/guides for the technologies they will be using.</t>
-  </si>
-  <si>
-    <t>3.4. Support and information to answer learner questions is available</t>
-  </si>
-  <si>
-    <t>3.4.1. Answers to common questions (e.g. Q&amp;A, FAQ) and/or a support-focused discussion forum are provided.</t>
-  </si>
-  <si>
-    <t>3.4.2. All necessary contact details for the teaching team (e.g. name, email, telephone, office location) are provided.</t>
   </si>
   <si>
     <r>
@@ -566,42 +454,13 @@
     </r>
   </si>
   <si>
-    <t>3.4.3. Information on availability of the teaching team is provided.</t>
-  </si>
-  <si>
-    <t>3.4.4. Information on ways to communicate with the teaching team is provided.</t>
-  </si>
-  <si>
-    <r>
-      <t>3.4.5. information about response timeframe</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> expectations is provided.</t>
-    </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">CBP </t>
     </r>
@@ -611,6 +470,7 @@
         <sz val="9"/>
         <color rgb="FF70AD47"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">RLST </t>
     </r>
@@ -620,57 +480,10 @@
         <sz val="9"/>
         <color rgb="FFFFC000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>CE</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">3.5. Learning analytics are available to learners. </t>
-  </si>
-  <si>
-    <t>3.5.1. Learners are able to access analytics (e.g. via a dashboard).</t>
-  </si>
-  <si>
-    <t>3.5.2. Learners are able to track their own learning progress using analytics.</t>
-  </si>
-  <si>
-    <t>3.5.3. Information on how to interpret learning analytics is provided.</t>
-  </si>
-  <si>
-    <t>4.1. Opportunities for learner-to-learner interactions are provided.</t>
-  </si>
-  <si>
-    <t>4.1.1. Opportunities and tools for both synchronous and asynchronous communication between learners are provided.</t>
-  </si>
-  <si>
-    <t>4.1.2. Opportunities and tools for learners to collaborate with each other are provided.</t>
-  </si>
-  <si>
-    <t>4.1.3. The intention of the learner-to-learner interaction (e.g. discussion forum - general or specific) is specified.</t>
-  </si>
-  <si>
-    <t>4.1.4. Learner-to-learner interaction expectations (e.g. scope and frequency and/or Netiquette) are provided.</t>
-  </si>
-  <si>
-    <t>4.2. Opportunities for learner-to-teacher interactions are provided.</t>
-  </si>
-  <si>
-    <t>4.2.1. Opportunities and tools for both synchronous and asynchronous communication between learners(s) and teacher(s) are provided.</t>
-  </si>
-  <si>
-    <t>4.2.2. Opportunities for both public and private/direct communication between learners and teachers are provided.</t>
-  </si>
-  <si>
-    <t>4.2.3. The intention of the learner-to-teacher interaction is specified.</t>
-  </si>
-  <si>
-    <t>4.2.4. Learner-to-teacher interaction expectations (e.g. scope and frequency and/or Netiquette) are provided.</t>
-  </si>
-  <si>
-    <t>4.3. There are explicit activities to develop and foster the learning community as well as establish relationships and connections are provided.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.3.1. Requirements for learner participation in the online environment are provided. </t>
   </si>
   <si>
     <r>
@@ -700,15 +513,13 @@
     </r>
   </si>
   <si>
-    <t>4.3.2. An activity requiring learners to introduce themselves to the learning community (can be synchronous or asynchronous) is provided.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
         <sz val="9"/>
         <color rgb="FF70AD47"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>RLST</t>
     </r>
@@ -718,15 +529,10 @@
         <sz val="9"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> RLSP</t>
     </r>
-  </si>
-  <si>
-    <t>4.3.3. A welcome message (e.g. text or video) is provided.</t>
-  </si>
-  <si>
-    <t>4.3.4. The teaching team is introduced (e.g. bios, video, Q&amp;A).</t>
   </si>
   <si>
     <r>
@@ -747,12 +553,6 @@
       </rPr>
       <t>RLST</t>
     </r>
-  </si>
-  <si>
-    <t>5.1. The aims, learning outcomes, schedule of learning and assessment tasks, and participation expectations are provided.</t>
-  </si>
-  <si>
-    <t>5.1.1. The aims, learning outcomes, participation expectations and assessment tasks are provided.</t>
   </si>
   <si>
     <r>
@@ -804,9 +604,6 @@
     </r>
   </si>
   <si>
-    <t>5.1.2. A schedule of the learning and assessment tasks is provided.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">CBP </t>
     </r>
@@ -845,31 +642,7 @@
     </r>
   </si>
   <si>
-    <t>5.2. Details of assessment tasks, their requirements, assessment criteria and feedback are provided.</t>
-  </si>
-  <si>
     <t>5.2.1 Assessment task details (e.g. type, weighting, size, nature of task/submission, requirements, approach) are provided.</t>
-  </si>
-  <si>
-    <t>5.2.2. Processes for assessment submission (method, mode, dates and times, linked to a specific time zone; as well as technical guidelines such as file upload format and size restrictions), handling, marking and feedback (including response times) are provided.</t>
-  </si>
-  <si>
-    <t>5.2.3. Assessment criteria (e.g. rubrics) for all tasks are provided.</t>
-  </si>
-  <si>
-    <t>5.2.4. Instructions on how and when originality checking software will be used are provided.</t>
-  </si>
-  <si>
-    <t>5.2.5. Assessment task examples (e.g. submissions by previous learners) are provided.</t>
-  </si>
-  <si>
-    <t>5.3. Expectations and outcomes for the learning and assessment tasks are provided.</t>
-  </si>
-  <si>
-    <t>5.3.1. Requirement for engagement with learning and assessment tasks is specified (e.g. essential or optional).</t>
-  </si>
-  <si>
-    <t>5.3.2. Expectations for extent of learner engagement in learning and assessment tasks are clearly stated (e.g. number of hours, length/depth of discussion).</t>
   </si>
   <si>
     <r>
@@ -888,94 +661,7 @@
     </r>
   </si>
   <si>
-    <t>5.4. Opportunities for learners to actively engage in a variety of learning and assessment tasks are provided.</t>
-  </si>
-  <si>
-    <t>5.4.1. Information is provided to learners to explain the connection between the learning and assessment tasks and their learning.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.4.2. Opportunities for learners to engage in a variety of tasks (e.g. co-creation, quizzes) are provided. </t>
-  </si>
-  <si>
-    <t>5.4.3. Opportunities for learners to engage independently and in collaboration with others (e.g. independent work, pairs, groups) are provided.</t>
-  </si>
-  <si>
-    <t>5.4.4. Opportunities for learners to respond in a variety of formats (e.g. presentation, written, audio, video) are provided.</t>
-  </si>
-  <si>
-    <t>5.4.5. Opportunities for learners to observe the work of others (e.g. peers, teachers, industry leaders) are provided.</t>
-  </si>
-  <si>
-    <t>5.5. Opportunities for learners to receive both formative and summative feedback are provided.</t>
-  </si>
-  <si>
-    <t>5.5.1. All opportunities for learners to receive feedback (e.g. automated, self, peer, teacher) are communicated.</t>
-  </si>
-  <si>
-    <t>5.5.2. Information about feedback (e.g. timing, format, interpretation, use) is provided.</t>
-  </si>
-  <si>
-    <t>6.1. Learning and assessment tasks are supported by relevant digital technology.</t>
-  </si>
-  <si>
-    <t>6.1.1. Learning and assessment tasks make effective use of technologies.</t>
-  </si>
-  <si>
-    <t>6.1.2. Learners are provided with instructions on how to use the tools/technology for learning and assessment tasks.</t>
-  </si>
-  <si>
-    <t>6.1.3. Where specific technologies are required, relevant access or directions to access the technologies (e.g. podcasting, blogs, graphics software) are provided.</t>
-  </si>
-  <si>
     <t>6.2 Opportunities to develop and demonstrate digital literacies are provided.</t>
-  </si>
-  <si>
-    <t>6.2.1. Learning and assessment tasks are designed so that learners with varying degrees of digital literacy can participate equitably.</t>
-  </si>
-  <si>
-    <t>6.2.2. Opportunities to develop and demonstrate digital literacies are appropriately scaffolded.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.1. Learning resources are available and functional. </t>
-  </si>
-  <si>
-    <t>7.1.1. Learning resources are available.</t>
-  </si>
-  <si>
-    <t>7.1.2. Learning resources to be downloaded or streamed are appropriately sized (e.g. large files/formats optimized/compressed where/when applicable).</t>
-  </si>
-  <si>
-    <t>7.1.3. Learning resources are functional on contemporary devices.</t>
-  </si>
-  <si>
-    <t>7.1.4. Learning resources enable learner control.</t>
-  </si>
-  <si>
-    <t>7.1.5. Learning resources are fit for purpose (e.g. any PDF form that learners are required to fill out online is editable).</t>
-  </si>
-  <si>
-    <t>7.2. Learning resources are copyright compliant and appropriately attributed.</t>
-  </si>
-  <si>
-    <t>7.2.1. Evidence is provided that copyright regulations have been observed.</t>
-  </si>
-  <si>
-    <t>7.2.2. Relevant levels of attribution (e.g. scholarly citations, Creative Commons) are provided.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.3. Learning resources reflect diversity. </t>
-  </si>
-  <si>
-    <t>7.3.1. Learning resources are culturally considerate (e.g. Indigenous/sensitive topic warning, inappropriate images/language not evident).</t>
-  </si>
-  <si>
-    <t>7.3.2. Learning resources reflect diversity including but not limited to gender, culture, demographic groups.</t>
-  </si>
-  <si>
-    <t>7.3.3. Learning resources are contextualized to more than one global region.</t>
-  </si>
-  <si>
-    <t>8.1. Learning resources are relevant.</t>
   </si>
   <si>
     <t>8.1.1 Context is provided for the learning resource (i.e. what it actually is, why it is relevant and essential or recommended).</t>
@@ -1008,15 +694,6 @@
     </r>
   </si>
   <si>
-    <t>8.2. Learning resources are provided in a range of modalities.</t>
-  </si>
-  <si>
-    <t>8.2.1. Learning resources utilise digital technologies and media (e.g. PDF, Video). in purposeful ways.</t>
-  </si>
-  <si>
-    <t>8.2.2. Learning resources are presented using a variety of technologies.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Your learning environment should be inclusive and function seamlessly across various devices, operating systems, and browsers. Ensure it meets contemporary accessibility standards and offers learners the opportunity to provide feedback at different stages.
 </t>
   </si>
@@ -1064,13 +741,331 @@
   </si>
   <si>
     <t>Learning resources are relevant and support learner engagement.</t>
+  </si>
+  <si>
+    <t>The online learning environment is inclusive.</t>
+  </si>
+  <si>
+    <t>Language used is consistently appropriate and inclusive (including consistent tone, voice, person).</t>
+  </si>
+  <si>
+    <t>The online learning environment contains evidence that diverse perspectives are respected.</t>
+  </si>
+  <si>
+    <t>The online learning environment functions across devices and platforms.</t>
+  </si>
+  <si>
+    <t>The online learning environment and integrated technology are compatible with contemporary browsers.</t>
+  </si>
+  <si>
+    <t>Online learning environment meets appropriate accessibility standards.</t>
+  </si>
+  <si>
+    <t>Files are appropriately optimised for screen readers, consistently named, then labelled by type and size.</t>
+  </si>
+  <si>
+    <t>Learners have opportunities to provide feedback.</t>
+  </si>
+  <si>
+    <t>Learners are informed about how their feedback is going to be collected and used.</t>
+  </si>
+  <si>
+    <t>The navigation and layout of the online learning environment is functional, consistent and intuitive.</t>
+  </si>
+  <si>
+    <t>The navigation is useable and functional.</t>
+  </si>
+  <si>
+    <t>Instructions on how to navigate the site and where to find learning activities are provided.</t>
+  </si>
+  <si>
+    <t>When learners are directed to external resources it opens in a new window/tab</t>
+  </si>
+  <si>
+    <t>The online learning environment is logically sequenced and organised.</t>
+  </si>
+  <si>
+    <t>A summary is provided that gives an overview of the learning sequence/design.</t>
+  </si>
+  <si>
+    <t>The content is divided into manageable segments that are appropriately labelled.</t>
+  </si>
+  <si>
+    <t>The content is organised to enhance ease of navigation.</t>
+  </si>
+  <si>
+    <t>Links to relevant services, information and policies are provided.</t>
+  </si>
+  <si>
+    <t>Links to academic support services and resources are provided.</t>
+  </si>
+  <si>
+    <t>Clear instructions for accessing technical support resources are provided.</t>
+  </si>
+  <si>
+    <t>Clear instructions for accessing technical support contacts are provided.</t>
+  </si>
+  <si>
+    <t>Instructions for accessing technical support services and resources are easy to find.</t>
+  </si>
+  <si>
+    <t>Clear and consistent instructions/guides for using the technology are provided.</t>
+  </si>
+  <si>
+    <t>The minimum technologies required to be successful are specified.</t>
+  </si>
+  <si>
+    <t>Learners are provided with instructions/guides for the technologies they will be using.</t>
+  </si>
+  <si>
+    <t>Support and information to answer learner questions is available</t>
+  </si>
+  <si>
+    <t>Information on availability of the teaching team is provided.</t>
+  </si>
+  <si>
+    <t>Information on ways to communicate with the teaching team is provided.</t>
+  </si>
+  <si>
+    <t>information about response timeframes expectations is provided.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning analytics are available to learners. </t>
+  </si>
+  <si>
+    <t>Learners are able to track their own learning progress using analytics.</t>
+  </si>
+  <si>
+    <t>Information on how to interpret learning analytics is provided.</t>
+  </si>
+  <si>
+    <t>Opportunities for learner-to-learner interactions are provided.</t>
+  </si>
+  <si>
+    <t>Opportunities and tools for both synchronous and asynchronous communication between learners are provided.</t>
+  </si>
+  <si>
+    <t>Opportunities and tools for learners to collaborate with each other are provided.</t>
+  </si>
+  <si>
+    <t>Opportunities for learner-to-teacher interactions are provided.</t>
+  </si>
+  <si>
+    <t>Opportunities and tools for both synchronous and asynchronous communication between learners(s) and teacher(s) are provided.</t>
+  </si>
+  <si>
+    <t>Opportunities for both public and private/direct communication between learners and teachers are provided.</t>
+  </si>
+  <si>
+    <t>The intention of the learner-to-teacher interaction is specified.</t>
+  </si>
+  <si>
+    <t>There are explicit activities to develop and foster the learning community as well as establish relationships and connections are provided.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements for learner participation in the online environment are provided. </t>
+  </si>
+  <si>
+    <t>An activity requiring learners to introduce themselves to the learning community (can be synchronous or asynchronous) is provided.</t>
+  </si>
+  <si>
+    <t>The aims, learning outcomes, schedule of learning and assessment tasks, and participation expectations are provided.</t>
+  </si>
+  <si>
+    <t>The aims, learning outcomes, participation expectations and assessment tasks are provided.</t>
+  </si>
+  <si>
+    <t>A schedule of the learning and assessment tasks is provided.</t>
+  </si>
+  <si>
+    <t>Details of assessment tasks, their requirements, assessment criteria and feedback are provided.</t>
+  </si>
+  <si>
+    <t>Processes for assessment submission (method, mode, dates and times, linked to a specific time zone; as well as technical guidelines such as file upload format and size restrictions), handling, marking and feedback (including response times) are provided.</t>
+  </si>
+  <si>
+    <t>Instructions on how and when originality checking software will be used are provided.</t>
+  </si>
+  <si>
+    <t>Expectations and outcomes for the learning and assessment tasks are provided.</t>
+  </si>
+  <si>
+    <t>Opportunities for learners to actively engage in a variety of learning and assessment tasks are provided.</t>
+  </si>
+  <si>
+    <t>Information is provided to learners to explain the connection between the learning and assessment tasks and their learning.</t>
+  </si>
+  <si>
+    <t>Opportunities for learners to receive both formative and summative feedback are provided.</t>
+  </si>
+  <si>
+    <t>Learning and assessment tasks are supported by relevant digital technology.</t>
+  </si>
+  <si>
+    <t>Learning and assessment tasks make effective use of technologies.</t>
+  </si>
+  <si>
+    <t>Learners are provided with instructions on how to use the tools/technology for learning and assessment tasks.</t>
+  </si>
+  <si>
+    <t>Learning and assessment tasks are designed so that learners with varying degrees of digital literacy can participate equitably.</t>
+  </si>
+  <si>
+    <t>Opportunities to develop and demonstrate digital literacies are appropriately scaffolded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning resources are available and functional. </t>
+  </si>
+  <si>
+    <t>Learning resources are available.</t>
+  </si>
+  <si>
+    <t>Learning resources are functional on contemporary devices.</t>
+  </si>
+  <si>
+    <t>Learning resources enable learner control.</t>
+  </si>
+  <si>
+    <t>Learning resources are copyright compliant and appropriately attributed.</t>
+  </si>
+  <si>
+    <t>Evidence is provided that copyright regulations have been observed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning resources reflect diversity. </t>
+  </si>
+  <si>
+    <t>Learning resources reflect diversity including but not limited to gender, culture, demographic groups.</t>
+  </si>
+  <si>
+    <t>Learning resources are contextualized to more than one global region.</t>
+  </si>
+  <si>
+    <t>Learning resources are relevant.</t>
+  </si>
+  <si>
+    <t>Learning resources are provided in a range of modalities.</t>
+  </si>
+  <si>
+    <t>Learning resources are presented using a variety of technologies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The online learning environment is responsive across different contemporary devices (e.g. screen size adjusting automatically).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The online learning environment and integrated technology are compatible across multiple platforms and operating systems.</t>
+  </si>
+  <si>
+    <t>Site, content and activities meet a contemporary set of accessibility standards/guidelines (e.g. accessible font, contrasting colour).</t>
+  </si>
+  <si>
+    <t>External tools and applications adhere to accessibility standards (e.g. Turnitin, VoiceThread, Echo360, SPSS, Padlet).</t>
+  </si>
+  <si>
+    <t>Alternate formats are made available for multimedia (e.g. images and alternate texts, subtitling for video or audio, transcripts for video and audio).</t>
+  </si>
+  <si>
+    <t>Learners have opportunities to provide immediate feedback (e.g. thumbs up/down, stars, flagging).</t>
+  </si>
+  <si>
+    <t>Learners have opportunities to provide feedback at different points in time (e.g. surveys polls, signposting).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> There is a consistent style guide (e.g. heading hierarchies, bulleted or numbered lists are consistent and tables only used for data).</t>
+  </si>
+  <si>
+    <t>All links and embedded resources are functional (i.e. not dead).</t>
+  </si>
+  <si>
+    <t>The channel(s) of communication for learners is articulated (e.g. dates, notices, updates and reminders).</t>
+  </si>
+  <si>
+    <t>The sequence of learning (i.e. order/flow) is logical.</t>
+  </si>
+  <si>
+    <t>Links to up-to-date, relevant policies (e.g. academic integrity, copyright, assessment procedures) are provided.</t>
+  </si>
+  <si>
+    <t>Links to up-to-date, relevant institutional services (e.g. library, learner support) are provided.</t>
+  </si>
+  <si>
+    <t>Answers to common questions (e.g. Q&amp;A, FAQ) and/or a support-focused discussion forum are provided.</t>
+  </si>
+  <si>
+    <t>All necessary contact details for the teaching team (e.g. name, email, telephone, office location) are provided.</t>
+  </si>
+  <si>
+    <t>Learners are able to access analytics (e.g. via a dashboard).</t>
+  </si>
+  <si>
+    <t>The intention of the learner-to-learner interaction (e.g. discussion forum - general or specific) is specified.</t>
+  </si>
+  <si>
+    <t>Learner-to-learner interaction expectations (e.g. scope and frequency and/or Netiquette) are provided.</t>
+  </si>
+  <si>
+    <t>Learner-to-teacher interaction expectations (e.g. scope and frequency and/or Netiquette) are provided.</t>
+  </si>
+  <si>
+    <t>A welcome message (e.g. text or video) is provided.</t>
+  </si>
+  <si>
+    <t>The teaching team is introduced (e.g. bios, video, Q&amp;A).</t>
+  </si>
+  <si>
+    <t>Assessment criteria (e.g. rubrics) for all tasks are provided.</t>
+  </si>
+  <si>
+    <t>Assessment task examples (e.g. submissions by previous learners) are provided.</t>
+  </si>
+  <si>
+    <t>Requirement for engagement with learning and assessment tasks is specified (e.g. essential or optional).</t>
+  </si>
+  <si>
+    <t>Expectations for extent of learner engagement in learning and assessment tasks are clearly stated (e.g. number of hours, length/depth of discussion).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opportunities for learners to engage in a variety of tasks (e.g. co-creation, quizzes) are provided. </t>
+  </si>
+  <si>
+    <t>Opportunities for learners to engage independently and in collaboration with others (e.g. independent work, pairs, groups) are provided.</t>
+  </si>
+  <si>
+    <t>Opportunities for learners to respond in a variety of formats (e.g. presentation, written, audio, video) are provided.</t>
+  </si>
+  <si>
+    <t>Opportunities for learners to observe the work of others (e.g. peers, teachers, industry leaders) are provided.</t>
+  </si>
+  <si>
+    <t>All opportunities for learners to receive feedback (e.g. automated, self, peer, teacher) are communicated.</t>
+  </si>
+  <si>
+    <t>Information about feedback (e.g. timing, format, interpretation, use) is provided.</t>
+  </si>
+  <si>
+    <t>Where specific technologies are required, relevant access or directions to access the technologies (e.g. podcasting, blogs, graphics software) are provided.</t>
+  </si>
+  <si>
+    <t>Learning resources to be downloaded or streamed are appropriately sized (e.g. large files/formats optimized/compressed where/when applicable).</t>
+  </si>
+  <si>
+    <t>Learning resources are fit for purpose (e.g. any PDF form that learners are required to fill out online is editable).</t>
+  </si>
+  <si>
+    <t>Relevant levels of attribution (e.g. scholarly citations, Creative Commons) are provided.</t>
+  </si>
+  <si>
+    <t>Learning resources are culturally considerate (e.g. Indigenous/sensitive topic warning, inappropriate images/language not evident).</t>
+  </si>
+  <si>
+    <t>Learning resources utilise digital technologies and media (e.g. PDF, Video). in purposeful ways.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1095,13 +1090,6 @@
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="9"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1174,24 +1162,28 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF009999"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1206,6 +1198,7 @@
       <sz val="9"/>
       <color rgb="FF70AD47"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1236,6 +1229,7 @@
       <sz val="9"/>
       <color rgb="FFFF3399"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1286,21 +1280,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color rgb="FF467886"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1571,13 +1562,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1611,128 +1602,128 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="5" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2092,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5334662-9413-C34F-BABB-F5B50512B303}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2140,1310 +2131,1368 @@
       <c r="L1" s="34"/>
     </row>
     <row r="2" spans="1:12" ht="42" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
-        <v>193</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="57" t="s">
+      <c r="A2" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="E2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="I2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="J2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="K2" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.2">
+      <c r="A3" s="60"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="G3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="34"/>
-    </row>
-    <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A3" s="61"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="6" t="s">
+      <c r="J3" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="K3" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="40" t="s">
+      <c r="L3" s="34"/>
+    </row>
+    <row r="4" spans="1:12" ht="42" x14ac:dyDescent="0.2">
+      <c r="A4" s="60"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="56"/>
+      <c r="E4" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="G4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="J4" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="34"/>
-    </row>
-    <row r="4" spans="1:12" ht="42" x14ac:dyDescent="0.2">
-      <c r="A4" s="61"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="57" t="s">
+      <c r="K4" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="7" t="s">
+      <c r="L4" s="34"/>
+    </row>
+    <row r="5" spans="1:12" ht="39" x14ac:dyDescent="0.2">
+      <c r="A5" s="60"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="G5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="41" t="s">
+      <c r="K5" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="L5" s="34"/>
+    </row>
+    <row r="6" spans="1:12" ht="77" x14ac:dyDescent="0.2">
+      <c r="A6" s="60"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="39" t="s">
+      <c r="G6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="34"/>
-    </row>
-    <row r="5" spans="1:12" ht="39" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="8" t="s">
+      <c r="J6" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="K6" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="39" t="s">
+      <c r="L6" s="34"/>
+    </row>
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A7" s="60"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="56"/>
+      <c r="E7" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="G7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="34"/>
-    </row>
-    <row r="6" spans="1:12" ht="77" x14ac:dyDescent="0.2">
-      <c r="A6" s="61"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="9" t="s">
+      <c r="J7" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="K7" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="43" t="s">
+      <c r="L7" s="34"/>
+    </row>
+    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="A8" s="60"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="G8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="I8" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="34"/>
-    </row>
-    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A7" s="61"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="57" t="s">
+      <c r="J8" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="10" t="s">
+      <c r="K8" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="L8" s="34"/>
+    </row>
+    <row r="9" spans="1:12" ht="78" x14ac:dyDescent="0.2">
+      <c r="A9" s="60"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="45" t="s">
+      <c r="G9" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="46" t="s">
+      <c r="K9" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="34"/>
-    </row>
-    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A8" s="61"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="8" t="s">
+      <c r="L9" s="34"/>
+    </row>
+    <row r="10" spans="1:12" ht="52" x14ac:dyDescent="0.2">
+      <c r="A10" s="60"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="G10" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="K10" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="L10" s="34"/>
+    </row>
+    <row r="11" spans="1:12" ht="42" x14ac:dyDescent="0.2">
+      <c r="A11" s="60"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="E11" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="48" t="s">
+      <c r="G11" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="34"/>
-    </row>
-    <row r="9" spans="1:12" ht="78" x14ac:dyDescent="0.2">
-      <c r="A9" s="61"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="8" t="s">
+    </row>
+    <row r="12" spans="1:12" ht="84" x14ac:dyDescent="0.2">
+      <c r="A12" s="60"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="G12" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="56" x14ac:dyDescent="0.2">
+      <c r="A13" s="64"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="49" t="s">
+      <c r="G13" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="56"/>
+      <c r="E14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="G14" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K9" s="48" t="s">
+    </row>
+    <row r="15" spans="1:12" ht="28" x14ac:dyDescent="0.2">
+      <c r="A15" s="60"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="34"/>
-    </row>
-    <row r="10" spans="1:12" ht="52" x14ac:dyDescent="0.2">
-      <c r="A10" s="61"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="9" t="s">
+      <c r="G15" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="35" t="s">
+    </row>
+    <row r="16" spans="1:12" ht="26" x14ac:dyDescent="0.2">
+      <c r="A16" s="60"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="39" t="s">
+      <c r="G16" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28" x14ac:dyDescent="0.2">
+      <c r="A17" s="60"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F17" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="K10" s="46" t="s">
+      <c r="G17" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+      <c r="A18" s="60"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="34"/>
-    </row>
-    <row r="11" spans="1:12" ht="42" x14ac:dyDescent="0.2">
-      <c r="A11" s="61"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="57" t="s">
+      <c r="F18" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="G18" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28" x14ac:dyDescent="0.2">
+      <c r="A19" s="60"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="G19" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="70" x14ac:dyDescent="0.2">
+      <c r="A20" s="60"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F20" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="G20" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+      <c r="A21" s="60"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="56"/>
+      <c r="E21" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G21" s="23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="84" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="11" t="s">
+    <row r="22" spans="1:7" ht="28" x14ac:dyDescent="0.2">
+      <c r="A22" s="60"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F22" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="G22" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="56" x14ac:dyDescent="0.2">
+      <c r="A23" s="60"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="56" x14ac:dyDescent="0.2">
-      <c r="A13" s="62"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="6" t="s">
+      <c r="G23" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="64"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="G24" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="76" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="56"/>
+      <c r="E25" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="60" t="s">
-        <v>194</v>
-      </c>
-      <c r="B14" s="65" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="28" x14ac:dyDescent="0.2">
-      <c r="A15" s="61"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="26" x14ac:dyDescent="0.2">
-      <c r="A16" s="61"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A17" s="61"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="42" x14ac:dyDescent="0.2">
-      <c r="A18" s="61"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A19" s="61"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="70" x14ac:dyDescent="0.2">
-      <c r="A20" s="61"/>
-      <c r="B20" s="66"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="42" x14ac:dyDescent="0.2">
-      <c r="A21" s="61"/>
-      <c r="B21" s="66"/>
-      <c r="C21" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="57"/>
-      <c r="E21" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A22" s="61"/>
-      <c r="B22" s="66"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="56" x14ac:dyDescent="0.2">
-      <c r="A23" s="61"/>
-      <c r="B23" s="66"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="60" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="65" t="s">
-        <v>187</v>
-      </c>
-      <c r="C25" s="57" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="57"/>
-      <c r="E25" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>96</v>
-      </c>
       <c r="G25" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A26" s="61"/>
-      <c r="B26" s="66"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="60"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
       <c r="E26" s="8" t="s">
-        <v>97</v>
+        <v>175</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="17" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="61"/>
-      <c r="B27" s="66"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
+      <c r="A27" s="60"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
       <c r="E27" s="9" t="s">
-        <v>98</v>
+        <v>176</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="17" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="61"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="57"/>
+      <c r="A28" s="60"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="56"/>
       <c r="E28" s="7" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="17" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="61"/>
-      <c r="B29" s="66"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
+      <c r="A29" s="60"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
       <c r="E29" s="9" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="17" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="61"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="57" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="57"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="56"/>
       <c r="E30" s="12" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="17" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="61"/>
-      <c r="B31" s="66"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
+      <c r="A31" s="60"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
       <c r="E31" s="11" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="17" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="61"/>
-      <c r="B32" s="66"/>
-      <c r="C32" s="57" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" s="57"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="56"/>
       <c r="E32" s="10" t="s">
-        <v>106</v>
+        <v>177</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A33" s="61"/>
-      <c r="B33" s="66"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="59"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="60"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="57"/>
       <c r="E33" s="8" t="s">
-        <v>107</v>
+        <v>178</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="17" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="61"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="57"/>
+      <c r="A34" s="60"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="56"/>
       <c r="E34" s="8" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="17" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="61"/>
-      <c r="B35" s="66"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
+      <c r="A35" s="60"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="57"/>
       <c r="E35" s="11" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="17" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="61"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="57"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="56"/>
       <c r="E36" s="6" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="23" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="61"/>
-      <c r="B37" s="66"/>
-      <c r="C37" s="57" t="s">
-        <v>113</v>
-      </c>
-      <c r="D37" s="59"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="57"/>
       <c r="E37" s="5" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="24" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="61"/>
-      <c r="B38" s="66"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="57"/>
+      <c r="A38" s="60"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="56"/>
       <c r="E38" s="11" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="24" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="62"/>
-      <c r="B39" s="67"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
+      <c r="A39" s="64"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
       <c r="E39" s="6" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="24" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="60" t="s">
-        <v>196</v>
-      </c>
-      <c r="B40" s="65" t="s">
-        <v>188</v>
-      </c>
-      <c r="C40" s="57" t="s">
-        <v>117</v>
-      </c>
-      <c r="D40" s="57"/>
+      <c r="A40" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="56"/>
       <c r="E40" s="5" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="25" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="61"/>
-      <c r="B41" s="66"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="59"/>
+      <c r="A41" s="60"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="57"/>
       <c r="E41" s="11" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="25" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="61"/>
-      <c r="B42" s="66"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="57"/>
+      <c r="A42" s="60"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="56"/>
       <c r="E42" s="11" t="s">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="25" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="61"/>
-      <c r="B43" s="66"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="59"/>
+      <c r="A43" s="60"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
       <c r="E43" s="6" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="25" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A44" s="61"/>
-      <c r="B44" s="66"/>
-      <c r="C44" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="57"/>
+      <c r="A44" s="60"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" s="56"/>
       <c r="E44" s="12" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A45" s="61"/>
-      <c r="B45" s="66"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="59"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="60"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="57"/>
       <c r="E45" s="11" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="F45" s="14"/>
       <c r="G45" s="26" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="61"/>
-      <c r="B46" s="66"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="57"/>
+      <c r="A46" s="60"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="56"/>
       <c r="E46" s="11" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F46" s="14"/>
       <c r="G46" s="26" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="61"/>
-      <c r="B47" s="66"/>
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
+      <c r="A47" s="60"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
       <c r="E47" s="6" t="s">
-        <v>126</v>
+        <v>182</v>
       </c>
       <c r="F47" s="14"/>
       <c r="G47" s="26" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="61"/>
-      <c r="B48" s="66"/>
-      <c r="C48" s="57" t="s">
-        <v>127</v>
-      </c>
-      <c r="D48" s="57"/>
+      <c r="A48" s="60"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" s="56"/>
       <c r="E48" s="12" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="F48" s="14"/>
       <c r="G48" s="27" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A49" s="61"/>
-      <c r="B49" s="66"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="59"/>
+      <c r="A49" s="60"/>
+      <c r="B49" s="55"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="57"/>
       <c r="E49" s="11" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F49" s="14"/>
       <c r="G49" s="28" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="61"/>
-      <c r="B50" s="66"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="57"/>
+      <c r="A50" s="60"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="56"/>
       <c r="E50" s="8" t="s">
-        <v>132</v>
+        <v>183</v>
       </c>
       <c r="F50" s="14"/>
       <c r="G50" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="62"/>
-      <c r="B51" s="67"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
+      <c r="A51" s="64"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
       <c r="E51" s="9" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="F51" s="14"/>
       <c r="G51" s="30" t="s">
-        <v>134</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="B52" s="65" t="s">
-        <v>189</v>
-      </c>
-      <c r="C52" s="57" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="57"/>
+      <c r="A52" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="56"/>
       <c r="E52" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F52" s="14"/>
       <c r="G52" s="17" t="s">
-        <v>137</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="61"/>
-      <c r="B53" s="66"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
+      <c r="A53" s="60"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
       <c r="E53" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="17" t="s">
-        <v>139</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A54" s="61"/>
-      <c r="B54" s="66"/>
-      <c r="C54" s="57" t="s">
+      <c r="A54" s="60"/>
+      <c r="B54" s="55"/>
+      <c r="C54" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="D54" s="57"/>
+      <c r="D54" s="56"/>
       <c r="E54" s="12" t="s">
-        <v>141</v>
+        <v>74</v>
       </c>
       <c r="F54" s="14"/>
       <c r="G54" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="39" x14ac:dyDescent="0.2">
-      <c r="A55" s="61"/>
-      <c r="B55" s="66"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="59"/>
+      <c r="A55" s="60"/>
+      <c r="B55" s="55"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="57"/>
       <c r="E55" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F55" s="14"/>
       <c r="G55" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="61"/>
-      <c r="B56" s="66"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="57"/>
+      <c r="A56" s="60"/>
+      <c r="B56" s="55"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="56"/>
       <c r="E56" s="8" t="s">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="F56" s="14"/>
       <c r="G56" s="17" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="61"/>
-      <c r="B57" s="66"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="59"/>
+      <c r="A57" s="60"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="57"/>
       <c r="E57" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F57" s="14"/>
       <c r="G57" s="20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="61"/>
-      <c r="B58" s="66"/>
-      <c r="C58" s="59"/>
-      <c r="D58" s="57"/>
+      <c r="A58" s="60"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="56"/>
       <c r="E58" s="6" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="F58" s="14"/>
       <c r="G58" s="31" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="61"/>
-      <c r="B59" s="66"/>
-      <c r="C59" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="D59" s="59"/>
+      <c r="A59" s="60"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="D59" s="57"/>
       <c r="E59" s="12" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="F59" s="14"/>
       <c r="G59" s="20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A60" s="61"/>
-      <c r="B60" s="66"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="57"/>
+      <c r="A60" s="60"/>
+      <c r="B60" s="55"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="56"/>
       <c r="E60" s="6" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
       <c r="F60" s="14"/>
       <c r="G60" s="17" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A61" s="61"/>
-      <c r="B61" s="66"/>
-      <c r="C61" s="57" t="s">
-        <v>150</v>
-      </c>
-      <c r="D61" s="59"/>
+      <c r="A61" s="60"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="D61" s="57"/>
       <c r="E61" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F61" s="14"/>
       <c r="G61" s="31" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="61"/>
-      <c r="B62" s="66"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="57"/>
+      <c r="A62" s="60"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="56"/>
       <c r="E62" s="11" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="F62" s="14"/>
       <c r="G62" s="31" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A63" s="61"/>
-      <c r="B63" s="66"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="59"/>
+      <c r="A63" s="60"/>
+      <c r="B63" s="55"/>
+      <c r="C63" s="61"/>
+      <c r="D63" s="57"/>
       <c r="E63" s="11" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="F63" s="14"/>
       <c r="G63" s="31" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A64" s="61"/>
-      <c r="B64" s="66"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="57"/>
+      <c r="A64" s="60"/>
+      <c r="B64" s="55"/>
+      <c r="C64" s="61"/>
+      <c r="D64" s="56"/>
       <c r="E64" s="11" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
       <c r="F64" s="14"/>
       <c r="G64" s="32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="26" x14ac:dyDescent="0.2">
-      <c r="A65" s="61"/>
-      <c r="B65" s="66"/>
-      <c r="C65" s="59"/>
-      <c r="D65" s="59"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="60"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
       <c r="E65" s="6" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="F65" s="14"/>
       <c r="G65" s="31" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="61"/>
-      <c r="B66" s="66"/>
-      <c r="C66" s="57" t="s">
-        <v>156</v>
-      </c>
-      <c r="D66" s="57"/>
+      <c r="A66" s="60"/>
+      <c r="B66" s="55"/>
+      <c r="C66" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="D66" s="56"/>
       <c r="E66" s="12" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="26" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="62"/>
-      <c r="B67" s="67"/>
-      <c r="C67" s="59"/>
-      <c r="D67" s="59"/>
+      <c r="A67" s="64"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="57"/>
       <c r="E67" s="9" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="F67" s="14"/>
       <c r="G67" s="20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="B68" s="65" t="s">
-        <v>190</v>
-      </c>
-      <c r="C68" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="D68" s="54"/>
+      <c r="A68" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="B68" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="62"/>
       <c r="E68" s="5" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="F68" s="14"/>
       <c r="G68" s="32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="61"/>
-      <c r="B69" s="66"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="55"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="60"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="61"/>
+      <c r="D69" s="66"/>
       <c r="E69" s="11" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="F69" s="14"/>
       <c r="G69" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="61"/>
-      <c r="B70" s="66"/>
-      <c r="C70" s="63"/>
-      <c r="D70" s="55"/>
+      <c r="A70" s="60"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="67"/>
+      <c r="D70" s="66"/>
       <c r="E70" s="6" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="F70" s="14"/>
       <c r="G70" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="61"/>
-      <c r="B71" s="66"/>
-      <c r="C71" s="64" t="s">
-        <v>163</v>
-      </c>
-      <c r="D71" s="55"/>
+      <c r="A71" s="60"/>
+      <c r="B71" s="55"/>
+      <c r="C71" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="66"/>
       <c r="E71" s="12" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="F71" s="14"/>
     </row>
     <row r="72" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="62"/>
-      <c r="B72" s="67"/>
-      <c r="C72" s="59"/>
-      <c r="D72" s="55"/>
+      <c r="A72" s="64"/>
+      <c r="B72" s="65"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="66"/>
       <c r="E72" s="6" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="F72" s="14"/>
     </row>
     <row r="73" spans="1:7" ht="76" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="60" t="s">
-        <v>199</v>
-      </c>
-      <c r="B73" s="65" t="s">
-        <v>191</v>
-      </c>
-      <c r="C73" s="57" t="s">
-        <v>166</v>
-      </c>
-      <c r="D73" s="55"/>
+      <c r="A73" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D73" s="66"/>
       <c r="E73" s="5" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="F73" s="14"/>
       <c r="G73" s="27" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="61"/>
-      <c r="B74" s="66"/>
-      <c r="C74" s="58"/>
-      <c r="D74" s="55"/>
+      <c r="A74" s="60"/>
+      <c r="B74" s="55"/>
+      <c r="C74" s="61"/>
+      <c r="D74" s="66"/>
       <c r="E74" s="8" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="F74" s="14"/>
       <c r="G74" s="18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="61"/>
-      <c r="B75" s="66"/>
-      <c r="C75" s="58"/>
-      <c r="D75" s="55"/>
+      <c r="A75" s="60"/>
+      <c r="B75" s="55"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="66"/>
       <c r="E75" s="8" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="F75" s="14"/>
       <c r="G75" s="18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="61"/>
-      <c r="B76" s="66"/>
-      <c r="C76" s="58"/>
-      <c r="D76" s="55"/>
+      <c r="A76" s="60"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="61"/>
+      <c r="D76" s="66"/>
       <c r="E76" s="11" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="F76" s="14"/>
       <c r="G76" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="61"/>
-      <c r="B77" s="66"/>
-      <c r="C77" s="59"/>
-      <c r="D77" s="56"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="60"/>
+      <c r="B77" s="55"/>
+      <c r="C77" s="57"/>
+      <c r="D77" s="63"/>
       <c r="E77" s="6" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="F77" s="14"/>
       <c r="G77" s="22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="61"/>
-      <c r="B78" s="66"/>
-      <c r="C78" s="57" t="s">
-        <v>172</v>
-      </c>
-      <c r="D78" s="57"/>
+      <c r="A78" s="60"/>
+      <c r="B78" s="55"/>
+      <c r="C78" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="D78" s="56"/>
       <c r="E78" s="7" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="F78" s="14"/>
       <c r="G78" s="33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="61"/>
-      <c r="B79" s="66"/>
-      <c r="C79" s="59"/>
-      <c r="D79" s="59"/>
+      <c r="A79" s="60"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="57"/>
+      <c r="D79" s="57"/>
       <c r="E79" s="6" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="F79" s="14"/>
     </row>
     <row r="80" spans="1:7" ht="28" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="61"/>
-      <c r="B80" s="66"/>
-      <c r="C80" s="57" t="s">
-        <v>175</v>
-      </c>
-      <c r="D80" s="54"/>
+      <c r="A80" s="60"/>
+      <c r="B80" s="55"/>
+      <c r="C80" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="D80" s="62"/>
       <c r="E80" s="12" t="s">
-        <v>176</v>
+        <v>199</v>
       </c>
       <c r="F80" s="14"/>
       <c r="G80" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="61"/>
-      <c r="B81" s="66"/>
-      <c r="C81" s="58"/>
-      <c r="D81" s="55"/>
+      <c r="A81" s="60"/>
+      <c r="B81" s="55"/>
+      <c r="C81" s="61"/>
+      <c r="D81" s="66"/>
       <c r="E81" s="11" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="F81" s="14"/>
       <c r="G81" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="62"/>
-      <c r="B82" s="67"/>
-      <c r="C82" s="59"/>
-      <c r="D82" s="55"/>
+      <c r="A82" s="64"/>
+      <c r="B82" s="65"/>
+      <c r="C82" s="57"/>
+      <c r="D82" s="66"/>
       <c r="E82" s="6" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="F82" s="14"/>
       <c r="G82" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="60" t="s">
-        <v>200</v>
-      </c>
-      <c r="B83" s="65" t="s">
-        <v>192</v>
+      <c r="A83" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="54" t="s">
+        <v>86</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="D83" s="51"/>
       <c r="E83" s="13" t="s">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="F83" s="14"/>
       <c r="G83" s="15" t="s">
-        <v>181</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="61"/>
-      <c r="B84" s="66"/>
-      <c r="C84" s="64" t="s">
-        <v>182</v>
-      </c>
-      <c r="D84" s="54"/>
+      <c r="A84" s="60"/>
+      <c r="B84" s="55"/>
+      <c r="C84" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="D84" s="62"/>
       <c r="E84" s="12" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="F84" s="14"/>
     </row>
     <row r="85" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="61"/>
-      <c r="B85" s="66"/>
-      <c r="C85" s="59"/>
-      <c r="D85" s="56"/>
+      <c r="A85" s="60"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="57"/>
+      <c r="D85" s="63"/>
       <c r="E85" s="11" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F85" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="D73:D77"/>
+    <mergeCell ref="D80:D82"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="A14:A24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A25:A39"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="B14:B24"/>
+    <mergeCell ref="B25:B39"/>
+    <mergeCell ref="A40:A51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C61:C65"/>
+    <mergeCell ref="A52:A67"/>
+    <mergeCell ref="B40:B51"/>
+    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C73:C77"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="A73:A82"/>
+    <mergeCell ref="B52:B67"/>
+    <mergeCell ref="B68:B72"/>
+    <mergeCell ref="B73:B82"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D20"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D84:D85"/>
     <mergeCell ref="B83:B85"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="D66:D67"/>
@@ -3460,64 +3509,6 @@
     <mergeCell ref="D60:D61"/>
     <mergeCell ref="D62:D63"/>
     <mergeCell ref="D64:D65"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D20"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="A68:A72"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C73:C77"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="A73:A82"/>
-    <mergeCell ref="B52:B67"/>
-    <mergeCell ref="B68:B72"/>
-    <mergeCell ref="B73:B82"/>
-    <mergeCell ref="A40:A51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C61:C65"/>
-    <mergeCell ref="A52:A67"/>
-    <mergeCell ref="B40:B51"/>
-    <mergeCell ref="A14:A24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A25:A39"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="B14:B24"/>
-    <mergeCell ref="B25:B39"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="D73:D77"/>
-    <mergeCell ref="D80:D82"/>
-    <mergeCell ref="C14:C20"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K6" r:id="rId1" display="Involves authentic learning – the use of examples that connect students to the material. See https://teachwell.auckland.ac.nz/signature-pedagogies/relational-learning/students-subjects/" xr:uid="{C079F0DD-4AAD-4699-887D-CCCBEC1D9D4C}"/>

</xml_diff>